<commit_message>
Updated DataValidation_Schema_Stats.py and utils.py
</commit_message>
<xml_diff>
--- a/temp_messy_transactions_20190103_20241231.xlsx
+++ b/temp_messy_transactions_20190103_20241231.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\MLOps\SupplyChainOptimization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A611B2DD-F187-414A-938A-B8D00C46966F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70ADA2D3-6FA3-42D7-BA91-D0FC789643EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CFABC2B5-CF00-4A99-A52D-F72273C9D635}"/>
   </bookViews>
@@ -567,7 +567,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>